<commit_message>
Extended Excel files reading
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\myseleniumshowtime\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F403BC1-B356-4DF2-A99E-31EF26CEA133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3886C882-4EF5-4E0B-B186-E2F9DDBF3F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -34,6 +30,9 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -364,7 +363,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,8 +385,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TDD via Excel file, fixed errors with parsing .xmlx file
</commit_message>
<xml_diff>
--- a/excel/data.xlsx
+++ b/excel/data.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3886C882-4EF5-4E0B-B186-E2F9DDBF3F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\myseleniumshowtime\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A888CC94-3407-428B-853D-519F579406DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -32,7 +36,19 @@
     <t>Admin</t>
   </si>
   <si>
+    <t>Admin2</t>
+  </si>
+  <si>
+    <t>Admin3</t>
+  </si>
+  <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>admin1234</t>
+  </si>
+  <si>
+    <t>admin12345</t>
   </si>
 </sst>
 </file>
@@ -360,17 +376,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -386,7 +401,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>